<commit_message>
mapping multiple  Montana nces schools to single acfr
</commit_message>
<xml_diff>
--- a/data/_dictionary_montana_school_districts.xlsx
+++ b/data/_dictionary_montana_school_districts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C05CB4D-52FD-2645-A01F-C69950C943E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB59798-DAE3-D148-8F85-B4C3B8E3AC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21060" yWindow="5560" windowWidth="27240" windowHeight="16440" xr2:uid="{F83193FE-6F4D-FC41-9B78-6309FC4C2D5F}"/>
+    <workbookView xWindow="17560" yWindow="5560" windowWidth="27240" windowHeight="16440" xr2:uid="{F83193FE-6F4D-FC41-9B78-6309FC4C2D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
   <si>
     <t>billings elem</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>Kalispell Public Schools</t>
-  </si>
-  <si>
-    <t>flathead h s</t>
-  </si>
-  <si>
-    <t>3015420</t>
   </si>
   <si>
     <t>butte elem</t>
@@ -649,7 +643,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -660,25 +654,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -828,28 +822,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9">
-        <v>35401</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
@@ -858,18 +838,18 @@
         <v>2</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>46750</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
@@ -884,12 +864,12 @@
         <v>35403</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>1</v>
@@ -898,21 +878,21 @@
         <v>2</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>35403</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>1</v>
@@ -921,18 +901,18 @@
         <v>2</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13">
         <v>586625</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>1</v>
@@ -947,12 +927,12 @@
         <v>586625</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>1</v>
@@ -961,18 +941,18 @@
         <v>2</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>35418</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>1</v>
@@ -981,18 +961,18 @@
         <v>2</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>35417</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>1</v>
@@ -1001,18 +981,18 @@
         <v>2</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>35402</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -1027,12 +1007,12 @@
         <v>35402</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>1</v>
@@ -1041,18 +1021,18 @@
         <v>2</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E19">
         <v>46750</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -1061,18 +1041,18 @@
         <v>2</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E20">
         <v>42164</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>1</v>
@@ -1087,12 +1067,12 @@
         <v>42164</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>1</v>
@@ -1107,12 +1087,12 @@
         <v>43285</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>1</v>
@@ -1121,18 +1101,18 @@
         <v>2</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E23">
         <v>43285</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>1</v>
@@ -1141,18 +1121,18 @@
         <v>2</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E24">
         <v>43827</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -1167,7 +1147,7 @@
         <v>43827</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>